<commit_message>
Updates for the final delivery
</commit_message>
<xml_diff>
--- a/data/interim/Conversion_factors.xlsx
+++ b/data/interim/Conversion_factors.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\Downloads\Python basics\Project_V3\Python stuff\Thesis2024\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10B5438-771A-4E46-9694-C1725E709E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{AECABF20-05DE-4B30-904B-997D38FBFD08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion factors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Conversion factors'!$A$1:$E$261</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,35 +38,62 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={DA395E04-3F60-4DA0-8EE6-CDFE4ABF07F1}</author>
     <author>tc={B6431F2D-DBB6-41DB-9933-40FDC0D54C7E}</author>
     <author>tc={0696B278-AC1C-44CB-97B4-98914DA8A600}</author>
   </authors>
   <commentList>
-    <comment ref="C89" authorId="0" shapeId="0" xr:uid="{DA395E04-3F60-4DA0-8EE6-CDFE4ABF07F1}">
+    <comment ref="C89" authorId="0" shapeId="0">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     This involves around 5 spring onions. Some recepies mention this ingredient as a cup full of spring onions chopped, some others mentioned bunch as a unit.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C94" authorId="1" shapeId="0" xr:uid="{B6431F2D-DBB6-41DB-9933-40FDC0D54C7E}">
+    <comment ref="C94" authorId="1" shapeId="0">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Including the stalk</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C98" authorId="2" shapeId="0" xr:uid="{0696B278-AC1C-44CB-97B4-98914DA8A600}">
+    <comment ref="C98" authorId="2" shapeId="0">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1 head of a mature Pakchoi</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -73,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="301">
   <si>
     <t>Ingredient</t>
   </si>
@@ -958,13 +986,31 @@
   </si>
   <si>
     <t>https://coolconversion.com/cooking-volume-weight/1~tbsp~of~canola+oil~to~gram</t>
+  </si>
+  <si>
+    <t>Nutritional yeast</t>
+  </si>
+  <si>
+    <t>Broth vegetables</t>
+  </si>
+  <si>
+    <t>Broth beef</t>
+  </si>
+  <si>
+    <t>Broth poultry</t>
+  </si>
+  <si>
+    <t>Tomato paste</t>
+  </si>
+  <si>
+    <t>Butter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1376,23 +1422,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AD4DC9-0E31-41B9-A5F3-F74C564CEEA9}">
-  <dimension ref="A1:J264"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F259" sqref="F116:F259"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" customWidth="1"/>
+    <col min="3" max="3" width="7.375" customWidth="1"/>
+    <col min="4" max="4" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1457,7 @@
       <c r="G1" s="1"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -1430,7 +1476,7 @@
       <c r="G2" s="1"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -1449,7 +1495,7 @@
       <c r="G3" s="1"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -1468,7 +1514,7 @@
       <c r="G4" s="1"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -1487,7 +1533,7 @@
       <c r="G5" s="1"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -1506,7 +1552,7 @@
       <c r="G6" s="1"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1525,7 +1571,7 @@
       <c r="G7" s="1"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -1544,7 +1590,7 @@
       <c r="G8" s="1"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -1563,7 +1609,7 @@
       <c r="G9" s="1"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1582,7 +1628,7 @@
       <c r="G10" s="1"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" t="s">
         <v>106</v>
       </c>
@@ -1601,7 +1647,7 @@
       <c r="G11" s="1"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" t="s">
         <v>107</v>
       </c>
@@ -1620,7 +1666,7 @@
       <c r="G12" s="1"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -1639,7 +1685,7 @@
       <c r="G13" s="1"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" t="s">
         <v>109</v>
       </c>
@@ -1658,7 +1704,7 @@
       <c r="G14" s="1"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -1677,7 +1723,7 @@
       <c r="G15" s="1"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -1696,7 +1742,7 @@
       <c r="G16" s="1"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -1715,7 +1761,7 @@
       <c r="G17" s="1"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -1734,7 +1780,7 @@
       <c r="G18" s="1"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -1753,7 +1799,7 @@
       <c r="G19" s="1"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -1772,7 +1818,7 @@
       <c r="G20" s="1"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -1791,7 +1837,7 @@
       <c r="G21" s="1"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -1810,7 +1856,7 @@
       <c r="G22" s="1"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -1829,7 +1875,7 @@
       <c r="G23" s="1"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -1848,7 +1894,7 @@
       <c r="G24" s="1"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -1867,7 +1913,7 @@
       <c r="G25" s="1"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -1886,7 +1932,7 @@
       <c r="G26" s="1"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -1905,7 +1951,7 @@
       <c r="G27" s="1"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -1924,7 +1970,7 @@
       <c r="G28" s="1"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -1943,7 +1989,7 @@
       <c r="G29" s="1"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -1962,7 +2008,7 @@
       <c r="G30" s="1"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -1981,7 +2027,7 @@
       <c r="G31" s="1"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15">
       <c r="A32" t="s">
         <v>127</v>
       </c>
@@ -2000,7 +2046,7 @@
       <c r="G32" s="1"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -2019,7 +2065,7 @@
       <c r="G33" s="1"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15">
       <c r="A34" t="s">
         <v>129</v>
       </c>
@@ -2038,7 +2084,7 @@
       <c r="G34" s="1"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15">
       <c r="A35" t="s">
         <v>130</v>
       </c>
@@ -2057,7 +2103,7 @@
       <c r="G35" s="1"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15">
       <c r="A36" t="s">
         <v>131</v>
       </c>
@@ -2076,7 +2122,7 @@
       <c r="G36" s="1"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -2095,7 +2141,7 @@
       <c r="G37" s="1"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -2114,7 +2160,7 @@
       <c r="G38" s="1"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15">
       <c r="A39" t="s">
         <v>134</v>
       </c>
@@ -2133,7 +2179,7 @@
       <c r="G39" s="1"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15">
       <c r="A40" t="s">
         <v>135</v>
       </c>
@@ -2152,7 +2198,7 @@
       <c r="G40" s="1"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -2171,7 +2217,7 @@
       <c r="G41" s="1"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -2190,7 +2236,7 @@
       <c r="G42" s="1"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15">
       <c r="A43" t="s">
         <v>138</v>
       </c>
@@ -2209,7 +2255,7 @@
       <c r="G43" s="1"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15">
       <c r="A44" t="s">
         <v>139</v>
       </c>
@@ -2228,7 +2274,7 @@
       <c r="G44" s="1"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15">
       <c r="A45" t="s">
         <v>140</v>
       </c>
@@ -2247,7 +2293,7 @@
       <c r="G45" s="1"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15">
       <c r="A46" t="s">
         <v>141</v>
       </c>
@@ -2266,7 +2312,7 @@
       <c r="G46" s="1"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -2285,7 +2331,7 @@
       <c r="G47" s="1"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15">
       <c r="A48" t="s">
         <v>143</v>
       </c>
@@ -2304,7 +2350,7 @@
       <c r="G48" s="1"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -2323,7 +2369,7 @@
       <c r="G49" s="1"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15">
       <c r="A50" t="s">
         <v>145</v>
       </c>
@@ -2342,7 +2388,7 @@
       <c r="G50" s="1"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15">
       <c r="A51" t="s">
         <v>146</v>
       </c>
@@ -2361,7 +2407,7 @@
       <c r="G51" s="1"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="14.25" customHeight="1">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -2380,7 +2426,7 @@
       <c r="G52" s="1"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="14.25" customHeight="1">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -2399,7 +2445,7 @@
       <c r="G53" s="1"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15">
       <c r="A54" t="s">
         <v>148</v>
       </c>
@@ -2418,7 +2464,7 @@
       <c r="G54" s="1"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15">
       <c r="A55" t="s">
         <v>149</v>
       </c>
@@ -2437,7 +2483,7 @@
       <c r="G55" s="1"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="15">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2456,7 +2502,7 @@
       <c r="G56" s="1"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -2475,7 +2521,7 @@
       <c r="G57" s="1"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="15">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -2494,7 +2540,7 @@
       <c r="G58" s="1"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15">
       <c r="A59" t="s">
         <v>150</v>
       </c>
@@ -2513,7 +2559,7 @@
       <c r="G59" s="1"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -2532,7 +2578,7 @@
       <c r="G60" s="1"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -2551,7 +2597,7 @@
       <c r="G61" s="1"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15">
       <c r="A62" t="s">
         <v>151</v>
       </c>
@@ -2570,7 +2616,7 @@
       <c r="G62" s="1"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15">
       <c r="A63" t="s">
         <v>152</v>
       </c>
@@ -2589,7 +2635,7 @@
       <c r="G63" s="1"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15">
       <c r="A64" t="s">
         <v>153</v>
       </c>
@@ -2608,7 +2654,7 @@
       <c r="G64" s="1"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15">
       <c r="A65" t="s">
         <v>153</v>
       </c>
@@ -2627,7 +2673,7 @@
       <c r="G65" s="1"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15">
       <c r="A66" t="s">
         <v>154</v>
       </c>
@@ -2646,7 +2692,7 @@
       <c r="G66" s="1"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15">
       <c r="A67" t="s">
         <v>154</v>
       </c>
@@ -2665,7 +2711,7 @@
       <c r="G67" s="1"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15">
       <c r="A68" t="s">
         <v>9</v>
       </c>
@@ -2684,7 +2730,7 @@
       <c r="G68" s="1"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -2703,7 +2749,7 @@
       <c r="G69" s="1"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="15">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -2722,7 +2768,7 @@
       <c r="G70" s="1"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15">
       <c r="A71" t="s">
         <v>155</v>
       </c>
@@ -2741,7 +2787,7 @@
       <c r="G71" s="1"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15">
       <c r="A72" t="s">
         <v>156</v>
       </c>
@@ -2760,7 +2806,7 @@
       <c r="G72" s="1"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15">
       <c r="A73" t="s">
         <v>156</v>
       </c>
@@ -2779,7 +2825,7 @@
       <c r="G73" s="1"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15">
       <c r="A74" t="s">
         <v>157</v>
       </c>
@@ -2798,7 +2844,7 @@
       <c r="G74" s="1"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15">
       <c r="A75" t="s">
         <v>157</v>
       </c>
@@ -2817,7 +2863,7 @@
       <c r="G75" s="1"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15">
       <c r="A76" t="s">
         <v>158</v>
       </c>
@@ -2836,7 +2882,7 @@
       <c r="G76" s="1"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15">
       <c r="A77" t="s">
         <v>158</v>
       </c>
@@ -2855,7 +2901,7 @@
       <c r="G77" s="1"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2874,7 +2920,7 @@
       <c r="G78" s="1"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -2893,7 +2939,7 @@
       <c r="G79" s="1"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -2912,7 +2958,7 @@
       <c r="G80" s="1"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="15">
       <c r="A81" t="s">
         <v>159</v>
       </c>
@@ -2931,7 +2977,7 @@
       <c r="G81" s="1"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="15">
       <c r="A82" t="s">
         <v>21</v>
       </c>
@@ -2950,7 +2996,7 @@
       <c r="G82" s="1"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="15">
       <c r="A83" t="s">
         <v>23</v>
       </c>
@@ -2969,7 +3015,7 @@
       <c r="G83" s="1"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="15">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -2988,7 +3034,7 @@
       <c r="G84" s="1"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="15">
       <c r="A85" t="s">
         <v>25</v>
       </c>
@@ -3007,7 +3053,7 @@
       <c r="G85" s="1"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="15">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -3026,7 +3072,7 @@
       <c r="G86" s="1"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15">
       <c r="A87" t="s">
         <v>28</v>
       </c>
@@ -3045,7 +3091,7 @@
       <c r="G87" s="1"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="15">
       <c r="A88" t="s">
         <v>30</v>
       </c>
@@ -3064,7 +3110,7 @@
       <c r="G88" s="1"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="15">
       <c r="A89" t="s">
         <v>32</v>
       </c>
@@ -3083,7 +3129,7 @@
       <c r="G89" s="1"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="15">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -3102,7 +3148,7 @@
       <c r="G90" s="1"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="15">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -3121,7 +3167,7 @@
       <c r="G91" s="1"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="15">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -3140,7 +3186,7 @@
       <c r="G92" s="1"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="15">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -3159,7 +3205,7 @@
       <c r="G93" s="1"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="15">
       <c r="A94" t="s">
         <v>35</v>
       </c>
@@ -3178,7 +3224,7 @@
       <c r="G94" s="1"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="15">
       <c r="A95" t="s">
         <v>37</v>
       </c>
@@ -3197,7 +3243,7 @@
       <c r="G95" s="1"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="15">
       <c r="A96" t="s">
         <v>39</v>
       </c>
@@ -3216,7 +3262,7 @@
       <c r="G96" s="1"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="15">
       <c r="A97" t="s">
         <v>41</v>
       </c>
@@ -3235,7 +3281,7 @@
       <c r="G97" s="1"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="15">
       <c r="A98" t="s">
         <v>43</v>
       </c>
@@ -3254,7 +3300,7 @@
       <c r="G98" s="1"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="15">
       <c r="A99" t="s">
         <v>45</v>
       </c>
@@ -3273,7 +3319,7 @@
       <c r="G99" s="1"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="15">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -3292,7 +3338,7 @@
       <c r="G100" s="1"/>
       <c r="J100" s="2"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="15">
       <c r="A101" t="s">
         <v>49</v>
       </c>
@@ -3311,7 +3357,7 @@
       <c r="G101" s="1"/>
       <c r="J101" s="2"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -3330,7 +3376,7 @@
       <c r="G102" s="1"/>
       <c r="J102" s="2"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="15">
       <c r="A103" t="s">
         <v>53</v>
       </c>
@@ -3349,7 +3395,7 @@
       <c r="G103" s="1"/>
       <c r="J103" s="2"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="15">
       <c r="A104" t="s">
         <v>54</v>
       </c>
@@ -3368,7 +3414,7 @@
       <c r="G104" s="1"/>
       <c r="J104" s="2"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="15">
       <c r="A105" t="s">
         <v>56</v>
       </c>
@@ -3387,7 +3433,7 @@
       <c r="G105" s="1"/>
       <c r="J105" s="2"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="15">
       <c r="A106" t="s">
         <v>58</v>
       </c>
@@ -3406,7 +3452,7 @@
       <c r="G106" s="1"/>
       <c r="J106" s="2"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="15">
       <c r="A107" t="s">
         <v>60</v>
       </c>
@@ -3425,7 +3471,7 @@
       <c r="G107" s="1"/>
       <c r="J107" s="2"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="15">
       <c r="A108" t="s">
         <v>61</v>
       </c>
@@ -3444,7 +3490,7 @@
       <c r="G108" s="1"/>
       <c r="J108" s="2"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="15">
       <c r="A109" t="s">
         <v>62</v>
       </c>
@@ -3463,7 +3509,7 @@
       <c r="G109" s="1"/>
       <c r="J109" s="2"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="15">
       <c r="A110" t="s">
         <v>63</v>
       </c>
@@ -3482,7 +3528,7 @@
       <c r="G110" s="1"/>
       <c r="J110" s="2"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="15">
       <c r="A111" t="s">
         <v>160</v>
       </c>
@@ -3498,7 +3544,7 @@
       <c r="G111" s="1"/>
       <c r="J111" s="2"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="15">
       <c r="A112" t="s">
         <v>161</v>
       </c>
@@ -3514,7 +3560,7 @@
       <c r="G112" s="1"/>
       <c r="J112" s="2"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="15">
       <c r="A113" t="s">
         <v>162</v>
       </c>
@@ -3530,7 +3576,7 @@
       <c r="G113" s="1"/>
       <c r="J113" s="2"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="15">
       <c r="A114" t="s">
         <v>163</v>
       </c>
@@ -3546,7 +3592,7 @@
       <c r="G114" s="1"/>
       <c r="J114" s="2"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="15">
       <c r="A115" t="s">
         <v>164</v>
       </c>
@@ -3562,7 +3608,7 @@
       <c r="G115" s="1"/>
       <c r="J115" s="2"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="15">
       <c r="A116" t="s">
         <v>165</v>
       </c>
@@ -3578,7 +3624,7 @@
       <c r="G116" s="1"/>
       <c r="J116" s="2"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="15">
       <c r="A117" t="s">
         <v>166</v>
       </c>
@@ -3594,7 +3640,7 @@
       <c r="G117" s="1"/>
       <c r="J117" s="2"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="15">
       <c r="A118" t="s">
         <v>64</v>
       </c>
@@ -3613,7 +3659,7 @@
       <c r="G118" s="1"/>
       <c r="J118" s="2"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="15">
       <c r="A119" t="s">
         <v>66</v>
       </c>
@@ -3632,7 +3678,7 @@
       <c r="G119" s="1"/>
       <c r="J119" s="2"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="15">
       <c r="A120" t="s">
         <v>68</v>
       </c>
@@ -3651,7 +3697,7 @@
       <c r="G120" s="1"/>
       <c r="J120" s="2"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="15">
       <c r="A121" t="s">
         <v>69</v>
       </c>
@@ -3670,7 +3716,7 @@
       <c r="G121" s="1"/>
       <c r="J121" s="2"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="15">
       <c r="A122" t="s">
         <v>71</v>
       </c>
@@ -3689,7 +3735,7 @@
       <c r="G122" s="1"/>
       <c r="J122" s="2"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="15">
       <c r="A123" t="s">
         <v>72</v>
       </c>
@@ -3708,7 +3754,7 @@
       <c r="G123" s="1"/>
       <c r="J123" s="2"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="15">
       <c r="A124" t="s">
         <v>73</v>
       </c>
@@ -3727,7 +3773,7 @@
       <c r="G124" s="1"/>
       <c r="J124" s="2"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="15">
       <c r="A125" t="s">
         <v>74</v>
       </c>
@@ -3746,7 +3792,7 @@
       <c r="G125" s="1"/>
       <c r="J125" s="2"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="15">
       <c r="A126" t="s">
         <v>76</v>
       </c>
@@ -3765,7 +3811,7 @@
       <c r="G126" s="1"/>
       <c r="J126" s="2"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="15">
       <c r="A127" t="s">
         <v>77</v>
       </c>
@@ -3784,7 +3830,7 @@
       <c r="G127" s="1"/>
       <c r="J127" s="2"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="15">
       <c r="A128" t="s">
         <v>167</v>
       </c>
@@ -3803,7 +3849,7 @@
       <c r="G128" s="1"/>
       <c r="J128" s="2"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" ht="15">
       <c r="A129" t="s">
         <v>168</v>
       </c>
@@ -3822,7 +3868,7 @@
       <c r="G129" s="1"/>
       <c r="J129" s="2"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="15">
       <c r="A130" t="s">
         <v>169</v>
       </c>
@@ -3841,7 +3887,7 @@
       <c r="G130" s="1"/>
       <c r="J130" s="2"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="15">
       <c r="A131" t="s">
         <v>78</v>
       </c>
@@ -3860,7 +3906,7 @@
       <c r="G131" s="1"/>
       <c r="J131" s="2"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="15">
       <c r="A132" t="s">
         <v>79</v>
       </c>
@@ -3879,7 +3925,7 @@
       <c r="G132" s="1"/>
       <c r="J132" s="2"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="15">
       <c r="A133" t="s">
         <v>81</v>
       </c>
@@ -3898,7 +3944,7 @@
       <c r="G133" s="1"/>
       <c r="J133" s="2"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="15">
       <c r="A134" t="s">
         <v>82</v>
       </c>
@@ -3917,7 +3963,7 @@
       <c r="G134" s="1"/>
       <c r="J134" s="2"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="15">
       <c r="A135" t="s">
         <v>83</v>
       </c>
@@ -3936,7 +3982,7 @@
       <c r="G135" s="1"/>
       <c r="J135" s="2"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="15">
       <c r="A136" t="s">
         <v>85</v>
       </c>
@@ -3955,7 +4001,7 @@
       <c r="G136" s="1"/>
       <c r="J136" s="2"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="15">
       <c r="A137" t="s">
         <v>170</v>
       </c>
@@ -3971,7 +4017,7 @@
       <c r="G137" s="1"/>
       <c r="J137" s="2"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" ht="15">
       <c r="A138" t="s">
         <v>86</v>
       </c>
@@ -3990,7 +4036,7 @@
       <c r="G138" s="1"/>
       <c r="J138" s="2"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="15">
       <c r="A139" t="s">
         <v>87</v>
       </c>
@@ -4009,7 +4055,7 @@
       <c r="G139" s="1"/>
       <c r="J139" s="2"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="15">
       <c r="A140" t="s">
         <v>88</v>
       </c>
@@ -4028,7 +4074,7 @@
       <c r="G140" s="1"/>
       <c r="J140" s="2"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="15">
       <c r="A141" t="s">
         <v>90</v>
       </c>
@@ -4047,7 +4093,7 @@
       <c r="G141" s="1"/>
       <c r="J141" s="2"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="15">
       <c r="A142" t="s">
         <v>91</v>
       </c>
@@ -4066,7 +4112,7 @@
       <c r="G142" s="1"/>
       <c r="J142" s="2"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="15">
       <c r="A143" t="s">
         <v>171</v>
       </c>
@@ -4082,7 +4128,7 @@
       <c r="G143" s="1"/>
       <c r="J143" s="2"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="15">
       <c r="A144" t="s">
         <v>172</v>
       </c>
@@ -4098,7 +4144,7 @@
       <c r="G144" s="1"/>
       <c r="J144" s="2"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="15">
       <c r="A145" t="s">
         <v>173</v>
       </c>
@@ -4114,7 +4160,7 @@
       <c r="G145" s="1"/>
       <c r="J145" s="2"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="15">
       <c r="A146" t="s">
         <v>174</v>
       </c>
@@ -4130,7 +4176,7 @@
       <c r="G146" s="1"/>
       <c r="J146" s="2"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" ht="15">
       <c r="A147" t="s">
         <v>175</v>
       </c>
@@ -4146,7 +4192,7 @@
       <c r="G147" s="1"/>
       <c r="J147" s="2"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" ht="15">
       <c r="A148" t="s">
         <v>176</v>
       </c>
@@ -4162,7 +4208,7 @@
       <c r="G148" s="1"/>
       <c r="J148" s="2"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" ht="15">
       <c r="A149" t="s">
         <v>177</v>
       </c>
@@ -4178,7 +4224,7 @@
       <c r="G149" s="1"/>
       <c r="J149" s="2"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" ht="15">
       <c r="A150" t="s">
         <v>178</v>
       </c>
@@ -4197,7 +4243,7 @@
       <c r="G150" s="1"/>
       <c r="J150" s="2"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" ht="15">
       <c r="A151" t="s">
         <v>13</v>
       </c>
@@ -4213,7 +4259,7 @@
       <c r="G151" s="1"/>
       <c r="J151" s="2"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" ht="15">
       <c r="A152" t="s">
         <v>179</v>
       </c>
@@ -4232,7 +4278,7 @@
       <c r="G152" s="1"/>
       <c r="J152" s="2"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="15">
       <c r="A153" t="s">
         <v>180</v>
       </c>
@@ -4251,7 +4297,7 @@
       <c r="G153" s="1"/>
       <c r="J153" s="2"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="15">
       <c r="A154" t="s">
         <v>181</v>
       </c>
@@ -4270,7 +4316,7 @@
       <c r="G154" s="1"/>
       <c r="J154" s="2"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" ht="15">
       <c r="A155" t="s">
         <v>182</v>
       </c>
@@ -4289,9 +4335,9 @@
       <c r="G155" s="1"/>
       <c r="J155" s="2"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" ht="15">
       <c r="A156" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -4308,28 +4354,25 @@
       <c r="G156" s="1"/>
       <c r="J156" s="2"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" ht="15">
       <c r="A157" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B157">
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="D157">
-        <v>100</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>288</v>
+        <v>9</v>
       </c>
       <c r="G157" s="1"/>
       <c r="J157" s="2"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" ht="15">
       <c r="A158" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B158">
         <v>1</v>
@@ -4346,9 +4389,9 @@
       <c r="G158" s="1"/>
       <c r="J158" s="2"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" ht="15">
       <c r="A159" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -4365,9 +4408,9 @@
       <c r="G159" s="1"/>
       <c r="J159" s="2"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" ht="15">
       <c r="A160" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -4384,9 +4427,9 @@
       <c r="G160" s="1"/>
       <c r="J160" s="2"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" ht="15">
       <c r="A161" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -4395,14 +4438,14 @@
         <v>7</v>
       </c>
       <c r="D161">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G161" s="1"/>
       <c r="J161" s="2"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" ht="15">
       <c r="A162" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B162">
         <v>1</v>
@@ -4419,82 +4462,76 @@
       <c r="G162" s="1"/>
       <c r="J162" s="2"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="15">
       <c r="A163" t="s">
-        <v>186</v>
+        <v>93</v>
       </c>
       <c r="B163">
         <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>272</v>
+        <v>18</v>
       </c>
       <c r="D163">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>288</v>
+        <v>94</v>
       </c>
       <c r="G163" s="1"/>
       <c r="J163" s="2"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" ht="15">
       <c r="A164" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B164">
         <v>1</v>
       </c>
       <c r="C164" t="s">
-        <v>272</v>
+        <v>18</v>
       </c>
       <c r="D164">
-        <v>100</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>288</v>
+        <v>80</v>
       </c>
       <c r="G164" s="1"/>
       <c r="J164" s="2"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="15">
       <c r="A165" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B165">
         <v>1</v>
       </c>
       <c r="C165" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D165">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="G165" s="1"/>
       <c r="J165" s="2"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" ht="15">
       <c r="A166" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B166">
         <v>1</v>
       </c>
       <c r="C166" t="s">
-        <v>272</v>
+        <v>18</v>
       </c>
       <c r="D166">
         <v>100</v>
       </c>
-      <c r="E166" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="G166" s="1"/>
       <c r="J166" s="2"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" ht="15">
       <c r="A167" t="s">
-        <v>93</v>
+        <v>192</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -4503,81 +4540,84 @@
         <v>18</v>
       </c>
       <c r="D167">
-        <v>50</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="G167" s="1"/>
       <c r="J167" s="2"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" ht="15">
       <c r="A168" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B168">
         <v>1</v>
       </c>
       <c r="C168" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D168">
-        <v>80</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G168" s="1"/>
       <c r="J168" s="2"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" ht="15">
       <c r="A169" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B169">
         <v>1</v>
       </c>
       <c r="C169" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D169">
-        <v>150</v>
+        <v>13.2</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G169" s="1"/>
       <c r="J169" s="2"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" ht="15">
       <c r="A170" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B170">
         <v>1</v>
       </c>
       <c r="C170" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D170">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G170" s="1"/>
       <c r="J170" s="2"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="15">
       <c r="A171" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B171">
         <v>1</v>
       </c>
       <c r="C171" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D171">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="G171" s="1"/>
       <c r="J171" s="2"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="15">
       <c r="A172" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -4586,17 +4626,14 @@
         <v>5</v>
       </c>
       <c r="D172">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E172" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G172" s="1"/>
       <c r="J172" s="2"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" ht="15">
       <c r="A173" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -4605,17 +4642,14 @@
         <v>7</v>
       </c>
       <c r="D173">
-        <v>13.2</v>
-      </c>
-      <c r="E173" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G173" s="1"/>
       <c r="J173" s="2"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" ht="15">
       <c r="A174" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -4629,9 +4663,9 @@
       <c r="G174" s="1"/>
       <c r="J174" s="2"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" ht="15">
       <c r="A175" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -4645,9 +4679,9 @@
       <c r="G175" s="1"/>
       <c r="J175" s="2"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" ht="15">
       <c r="A176" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B176">
         <v>1</v>
@@ -4661,9 +4695,9 @@
       <c r="G176" s="1"/>
       <c r="J176" s="2"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" ht="15">
       <c r="A177" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -4677,25 +4711,28 @@
       <c r="G177" s="1"/>
       <c r="J177" s="2"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>196</v>
+    <row r="178" spans="1:10" ht="15">
+      <c r="A178" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="B178">
         <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>5</v>
+        <v>272</v>
       </c>
       <c r="D178">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="G178" s="1"/>
       <c r="J178" s="2"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>196</v>
+    <row r="179" spans="1:10" ht="15">
+      <c r="A179" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -4704,14 +4741,15 @@
         <v>7</v>
       </c>
       <c r="D179">
-        <v>14</v>
-      </c>
+        <v>8.5</v>
+      </c>
+      <c r="E179" s="2"/>
       <c r="G179" s="1"/>
       <c r="J179" s="2"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" ht="15">
       <c r="A180" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B180">
         <v>1</v>
@@ -4720,14 +4758,17 @@
         <v>5</v>
       </c>
       <c r="D180">
-        <v>5</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G180" s="1"/>
       <c r="J180" s="2"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="15">
       <c r="A181" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -4736,52 +4777,49 @@
         <v>7</v>
       </c>
       <c r="D181">
-        <v>14</v>
+        <v>13.2</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G181" s="1"/>
       <c r="J181" s="2"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
-        <v>198</v>
+    <row r="182" spans="1:10" ht="15">
+      <c r="A182" t="s">
+        <v>200</v>
       </c>
       <c r="B182">
         <v>1</v>
       </c>
       <c r="C182" t="s">
-        <v>272</v>
+        <v>5</v>
       </c>
       <c r="D182">
-        <v>100</v>
-      </c>
-      <c r="E182" s="2" t="s">
-        <v>288</v>
+        <v>5</v>
       </c>
       <c r="G182" s="1"/>
       <c r="J182" s="2"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" ht="15">
       <c r="A183" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B183">
         <v>1</v>
       </c>
       <c r="C183" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D183">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G183" s="1"/>
       <c r="J183" s="2"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" ht="15">
       <c r="A184" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -4790,33 +4828,30 @@
         <v>7</v>
       </c>
       <c r="D184">
-        <v>13.2</v>
-      </c>
-      <c r="E184" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="G184" s="1"/>
       <c r="J184" s="2"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" ht="15">
       <c r="A185" t="s">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="B185">
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D185">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G185" s="1"/>
       <c r="J185" s="2"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" ht="15">
       <c r="A186" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -4825,14 +4860,14 @@
         <v>7</v>
       </c>
       <c r="D186">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G186" s="1"/>
       <c r="J186" s="2"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" ht="15">
       <c r="A187" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -4841,14 +4876,14 @@
         <v>7</v>
       </c>
       <c r="D187">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G187" s="1"/>
       <c r="J187" s="2"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" ht="15">
       <c r="A188" t="s">
-        <v>17</v>
+        <v>204</v>
       </c>
       <c r="B188">
         <v>1</v>
@@ -4857,14 +4892,14 @@
         <v>7</v>
       </c>
       <c r="D188">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G188" s="1"/>
       <c r="J188" s="2"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" ht="15">
       <c r="A189" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -4873,20 +4908,20 @@
         <v>7</v>
       </c>
       <c r="D189">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G189" s="1"/>
       <c r="J189" s="2"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>203</v>
+    <row r="190" spans="1:10" ht="15">
+      <c r="A190" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="B190">
         <v>1</v>
       </c>
       <c r="C190" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D190">
         <v>30</v>
@@ -4894,111 +4929,111 @@
       <c r="G190" s="1"/>
       <c r="J190" s="2"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>204</v>
+    <row r="191" spans="1:10" ht="15">
+      <c r="A191" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="B191">
         <v>1</v>
       </c>
       <c r="C191" t="s">
-        <v>7</v>
+        <v>274</v>
       </c>
       <c r="D191">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="G191" s="1"/>
       <c r="J191" s="2"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>205</v>
+    <row r="192" spans="1:10" ht="15">
+      <c r="A192" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="B192">
         <v>1</v>
       </c>
       <c r="C192" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="D192">
-        <v>25</v>
+        <v>100</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="G192" s="1"/>
       <c r="J192" s="2"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" ht="15">
       <c r="A193" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B193">
         <v>1</v>
       </c>
       <c r="C193" t="s">
-        <v>18</v>
+        <v>272</v>
       </c>
       <c r="D193">
-        <v>30</v>
+        <v>100</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="G193" s="1"/>
       <c r="J193" s="2"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A194" s="3" t="s">
-        <v>207</v>
+    <row r="194" spans="1:10" ht="15">
+      <c r="A194" t="s">
+        <v>210</v>
       </c>
       <c r="B194">
         <v>1</v>
       </c>
       <c r="C194" t="s">
-        <v>274</v>
+        <v>7</v>
       </c>
       <c r="D194">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="G194" s="1"/>
       <c r="J194" s="2"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="s">
-        <v>208</v>
+    <row r="195" spans="1:10" ht="15">
+      <c r="A195" t="s">
+        <v>211</v>
       </c>
       <c r="B195">
         <v>1</v>
       </c>
       <c r="C195" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="D195">
-        <v>100</v>
-      </c>
-      <c r="E195" s="2" t="s">
-        <v>288</v>
+        <v>15</v>
       </c>
       <c r="G195" s="1"/>
       <c r="J195" s="2"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A196" s="3" t="s">
-        <v>209</v>
+    <row r="196" spans="1:10" ht="15">
+      <c r="A196" t="s">
+        <v>212</v>
       </c>
       <c r="B196">
         <v>1</v>
       </c>
       <c r="C196" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="D196">
-        <v>100</v>
-      </c>
-      <c r="E196" s="2" t="s">
-        <v>288</v>
+        <v>15</v>
       </c>
       <c r="G196" s="1"/>
       <c r="J196" s="2"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="15">
       <c r="A197" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B197">
         <v>1</v>
@@ -5012,9 +5047,9 @@
       <c r="G197" s="1"/>
       <c r="J197" s="2"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" ht="15">
       <c r="A198" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B198">
         <v>1</v>
@@ -5023,14 +5058,14 @@
         <v>7</v>
       </c>
       <c r="D198">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G198" s="1"/>
       <c r="J198" s="2"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" ht="15">
       <c r="A199" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -5039,14 +5074,14 @@
         <v>7</v>
       </c>
       <c r="D199">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G199" s="1"/>
       <c r="J199" s="2"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" ht="15">
       <c r="A200" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B200">
         <v>1</v>
@@ -5055,14 +5090,14 @@
         <v>7</v>
       </c>
       <c r="D200">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G200" s="1"/>
       <c r="J200" s="2"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" ht="15">
       <c r="A201" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B201">
         <v>1</v>
@@ -5076,9 +5111,9 @@
       <c r="G201" s="1"/>
       <c r="J201" s="2"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" ht="15">
       <c r="A202" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B202">
         <v>1</v>
@@ -5092,9 +5127,9 @@
       <c r="G202" s="1"/>
       <c r="J202" s="2"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" ht="15">
       <c r="A203" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B203">
         <v>1</v>
@@ -5108,9 +5143,9 @@
       <c r="G203" s="1"/>
       <c r="J203" s="2"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" ht="15">
       <c r="A204" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -5124,9 +5159,9 @@
       <c r="G204" s="1"/>
       <c r="J204" s="2"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" ht="15">
       <c r="A205" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -5140,9 +5175,9 @@
       <c r="G205" s="1"/>
       <c r="J205" s="2"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" ht="15">
       <c r="A206" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B206">
         <v>1</v>
@@ -5156,9 +5191,9 @@
       <c r="G206" s="1"/>
       <c r="J206" s="2"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" ht="15">
       <c r="A207" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -5172,9 +5207,9 @@
       <c r="G207" s="1"/>
       <c r="J207" s="2"/>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" ht="15">
       <c r="A208" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -5188,9 +5223,9 @@
       <c r="G208" s="1"/>
       <c r="J208" s="2"/>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" ht="15">
       <c r="A209" t="s">
-        <v>222</v>
+        <v>299</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -5204,9 +5239,9 @@
       <c r="G209" s="1"/>
       <c r="J209" s="2"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" ht="15">
       <c r="A210" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B210">
         <v>1</v>
@@ -5220,9 +5255,9 @@
       <c r="G210" s="1"/>
       <c r="J210" s="2"/>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" ht="15">
       <c r="A211" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -5236,9 +5271,9 @@
       <c r="G211" s="1"/>
       <c r="J211" s="2"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" ht="15">
       <c r="A212" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -5252,9 +5287,9 @@
       <c r="G212" s="1"/>
       <c r="J212" s="2"/>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" ht="15">
       <c r="A213" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B213">
         <v>1</v>
@@ -5263,14 +5298,14 @@
         <v>7</v>
       </c>
       <c r="D213">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G213" s="1"/>
       <c r="J213" s="2"/>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" ht="15">
       <c r="A214" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B214">
         <v>1</v>
@@ -5279,14 +5314,14 @@
         <v>7</v>
       </c>
       <c r="D214">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G214" s="1"/>
       <c r="J214" s="2"/>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" ht="15">
       <c r="A215" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B215">
         <v>1</v>
@@ -5300,9 +5335,9 @@
       <c r="G215" s="1"/>
       <c r="J215" s="2"/>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" ht="15">
       <c r="A216" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B216">
         <v>1</v>
@@ -5316,25 +5351,28 @@
       <c r="G216" s="1"/>
       <c r="J216" s="2"/>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" ht="15">
       <c r="A217" t="s">
-        <v>230</v>
+        <v>95</v>
       </c>
       <c r="B217">
         <v>1</v>
       </c>
       <c r="C217" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="D217">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E217" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="G217" s="1"/>
       <c r="J217" s="2"/>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" ht="15">
       <c r="A218" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B218">
         <v>1</v>
@@ -5343,33 +5381,30 @@
         <v>7</v>
       </c>
       <c r="D218">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G218" s="1"/>
       <c r="J218" s="2"/>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" ht="15">
       <c r="A219" t="s">
-        <v>95</v>
+        <v>233</v>
       </c>
       <c r="B219">
         <v>1</v>
       </c>
       <c r="C219" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="D219">
-        <v>5</v>
-      </c>
-      <c r="E219" s="2" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="G219" s="1"/>
       <c r="J219" s="2"/>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" ht="15">
       <c r="A220" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -5378,14 +5413,14 @@
         <v>7</v>
       </c>
       <c r="D220">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G220" s="1"/>
       <c r="J220" s="2"/>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" ht="15">
       <c r="A221" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -5394,14 +5429,14 @@
         <v>7</v>
       </c>
       <c r="D221">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G221" s="1"/>
       <c r="J221" s="2"/>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" ht="15">
       <c r="A222" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -5415,9 +5450,9 @@
       <c r="G222" s="1"/>
       <c r="J222" s="2"/>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" ht="15">
       <c r="A223" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B223">
         <v>1</v>
@@ -5426,14 +5461,14 @@
         <v>7</v>
       </c>
       <c r="D223">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G223" s="1"/>
       <c r="J223" s="2"/>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" ht="15">
       <c r="A224" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B224">
         <v>1</v>
@@ -5447,9 +5482,9 @@
       <c r="G224" s="1"/>
       <c r="J224" s="2"/>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" ht="15">
       <c r="A225" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -5463,9 +5498,9 @@
       <c r="G225" s="1"/>
       <c r="J225" s="2"/>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" ht="15">
       <c r="A226" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B226">
         <v>1</v>
@@ -5479,9 +5514,9 @@
       <c r="G226" s="1"/>
       <c r="J226" s="2"/>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" ht="15">
       <c r="A227" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -5495,9 +5530,9 @@
       <c r="G227" s="1"/>
       <c r="J227" s="2"/>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" ht="15">
       <c r="A228" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B228">
         <v>1</v>
@@ -5511,9 +5546,9 @@
       <c r="G228" s="1"/>
       <c r="J228" s="2"/>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" ht="15">
       <c r="A229" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B229">
         <v>1</v>
@@ -5522,14 +5557,14 @@
         <v>7</v>
       </c>
       <c r="D229">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G229" s="1"/>
       <c r="J229" s="2"/>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" ht="15">
       <c r="A230" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B230">
         <v>1</v>
@@ -5538,14 +5573,14 @@
         <v>7</v>
       </c>
       <c r="D230">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G230" s="1"/>
       <c r="J230" s="2"/>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" ht="15">
       <c r="A231" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B231">
         <v>1</v>
@@ -5559,9 +5594,9 @@
       <c r="G231" s="1"/>
       <c r="J231" s="2"/>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" ht="15">
       <c r="A232" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B232">
         <v>1</v>
@@ -5570,14 +5605,14 @@
         <v>7</v>
       </c>
       <c r="D232">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G232" s="1"/>
       <c r="J232" s="2"/>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" ht="15">
       <c r="A233" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B233">
         <v>1</v>
@@ -5586,14 +5621,14 @@
         <v>7</v>
       </c>
       <c r="D233">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G233" s="1"/>
       <c r="J233" s="2"/>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" ht="15">
       <c r="A234" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B234">
         <v>1</v>
@@ -5607,9 +5642,9 @@
       <c r="G234" s="1"/>
       <c r="J234" s="2"/>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" ht="15">
       <c r="A235" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B235">
         <v>1</v>
@@ -5623,9 +5658,9 @@
       <c r="G235" s="1"/>
       <c r="J235" s="2"/>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" ht="15">
       <c r="A236" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B236">
         <v>1</v>
@@ -5634,14 +5669,14 @@
         <v>7</v>
       </c>
       <c r="D236">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G236" s="1"/>
       <c r="J236" s="2"/>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" ht="15">
       <c r="A237" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B237">
         <v>1</v>
@@ -5655,9 +5690,9 @@
       <c r="G237" s="1"/>
       <c r="J237" s="2"/>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" ht="15">
       <c r="A238" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B238">
         <v>1</v>
@@ -5671,9 +5706,9 @@
       <c r="G238" s="1"/>
       <c r="J238" s="2"/>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" ht="15">
       <c r="A239" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B239">
         <v>1</v>
@@ -5682,14 +5717,14 @@
         <v>7</v>
       </c>
       <c r="D239">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G239" s="1"/>
       <c r="J239" s="2"/>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" ht="15">
       <c r="A240" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B240">
         <v>1</v>
@@ -5698,14 +5733,14 @@
         <v>7</v>
       </c>
       <c r="D240">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G240" s="1"/>
       <c r="J240" s="2"/>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" ht="15">
       <c r="A241" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -5719,9 +5754,9 @@
       <c r="G241" s="1"/>
       <c r="J241" s="2"/>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" ht="15">
       <c r="A242" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B242">
         <v>1</v>
@@ -5735,9 +5770,9 @@
       <c r="G242" s="1"/>
       <c r="J242" s="2"/>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" ht="15">
       <c r="A243" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B243">
         <v>1</v>
@@ -5751,9 +5786,9 @@
       <c r="G243" s="1"/>
       <c r="J243" s="2"/>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" ht="15">
       <c r="A244" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B244">
         <v>1</v>
@@ -5767,25 +5802,25 @@
       <c r="G244" s="1"/>
       <c r="J244" s="2"/>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" ht="15">
       <c r="A245" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B245">
         <v>1</v>
       </c>
       <c r="C245" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D245">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G245" s="1"/>
       <c r="J245" s="2"/>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" ht="15">
       <c r="A246" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B246">
         <v>1</v>
@@ -5799,25 +5834,25 @@
       <c r="G246" s="1"/>
       <c r="J246" s="2"/>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" ht="15">
       <c r="A247" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B247">
         <v>1</v>
       </c>
       <c r="C247" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D247">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="G247" s="1"/>
       <c r="J247" s="2"/>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" ht="15">
       <c r="A248" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B248">
         <v>1</v>
@@ -5826,14 +5861,14 @@
         <v>7</v>
       </c>
       <c r="D248">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G248" s="1"/>
       <c r="J248" s="2"/>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" ht="15">
       <c r="A249" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B249">
         <v>1</v>
@@ -5842,46 +5877,52 @@
         <v>7</v>
       </c>
       <c r="D249">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G249" s="1"/>
       <c r="J249" s="2"/>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" ht="15">
       <c r="A250" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
       <c r="B250">
         <v>1</v>
       </c>
       <c r="C250" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="D250">
-        <v>15</v>
+        <v>100</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="G250" s="1"/>
       <c r="J250" s="2"/>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" ht="15">
       <c r="A251" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
       <c r="B251">
         <v>1</v>
       </c>
       <c r="C251" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="D251">
-        <v>15</v>
+        <v>100</v>
+      </c>
+      <c r="E251" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="G251" s="1"/>
       <c r="J251" s="2"/>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" ht="15">
       <c r="A252" t="s">
-        <v>264</v>
+        <v>298</v>
       </c>
       <c r="B252">
         <v>1</v>
@@ -5898,9 +5939,9 @@
       <c r="G252" s="1"/>
       <c r="J252" s="2"/>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" ht="15">
       <c r="A253" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -5917,9 +5958,9 @@
       <c r="G253" s="1"/>
       <c r="J253" s="2"/>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" ht="15">
       <c r="A254" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B254">
         <v>1</v>
@@ -5936,9 +5977,9 @@
       <c r="G254" s="1"/>
       <c r="J254" s="2"/>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" ht="15">
       <c r="A255" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -5955,9 +5996,9 @@
       <c r="G255" s="1"/>
       <c r="J255" s="2"/>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" ht="15">
       <c r="A256" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B256">
         <v>1</v>
@@ -5974,9 +6015,9 @@
       <c r="G256" s="1"/>
       <c r="J256" s="2"/>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" ht="15">
       <c r="A257" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B257">
         <v>1</v>
@@ -5993,70 +6034,88 @@
       <c r="G257" s="1"/>
       <c r="J257" s="2"/>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" ht="15">
       <c r="A258" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B258">
         <v>1</v>
       </c>
       <c r="C258" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="D258">
-        <v>20</v>
+        <v>100</v>
+      </c>
+      <c r="E258" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="G258" s="1"/>
       <c r="J258" s="2"/>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" ht="15">
       <c r="A259" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
       <c r="B259">
         <v>1</v>
       </c>
       <c r="C259" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="D259">
-        <v>100</v>
-      </c>
-      <c r="E259" s="2" t="s">
-        <v>288</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E259" s="2"/>
       <c r="G259" s="1"/>
       <c r="J259" s="2"/>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A260" s="1"/>
+    <row r="260" spans="1:10" ht="15">
+      <c r="A260" t="s">
+        <v>270</v>
+      </c>
+      <c r="B260">
+        <v>1</v>
+      </c>
+      <c r="C260" t="s">
+        <v>7</v>
+      </c>
+      <c r="D260">
+        <v>20</v>
+      </c>
       <c r="G260" s="1"/>
       <c r="J260" s="2"/>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A261" s="1"/>
+    <row r="261" spans="1:10" ht="15">
+      <c r="A261" t="s">
+        <v>271</v>
+      </c>
+      <c r="B261">
+        <v>1</v>
+      </c>
+      <c r="C261" t="s">
+        <v>272</v>
+      </c>
+      <c r="D261">
+        <v>100</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="G261" s="1"/>
       <c r="J261" s="2"/>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" ht="15">
       <c r="A262" s="1"/>
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
-      <c r="D262" s="1"/>
-      <c r="E262" s="1"/>
       <c r="G262" s="1"/>
       <c r="J262" s="2"/>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" ht="15">
       <c r="A263" s="1"/>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
-      <c r="D263" s="1"/>
-      <c r="E263" s="1"/>
       <c r="G263" s="1"/>
       <c r="J263" s="2"/>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" ht="15">
       <c r="A264" s="1"/>
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
@@ -6065,153 +6124,169 @@
       <c r="G264" s="1"/>
       <c r="J264" s="2"/>
     </row>
+    <row r="265" spans="1:10" ht="15">
+      <c r="A265" s="1"/>
+      <c r="B265" s="1"/>
+      <c r="C265" s="1"/>
+      <c r="D265" s="1"/>
+      <c r="E265" s="1"/>
+      <c r="G265" s="1"/>
+      <c r="J265" s="2"/>
+    </row>
+    <row r="266" spans="1:10" ht="15">
+      <c r="A266" s="1"/>
+      <c r="B266" s="1"/>
+      <c r="C266" s="1"/>
+      <c r="D266" s="1"/>
+      <c r="E266" s="1"/>
+      <c r="G266" s="1"/>
+      <c r="J266" s="2"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E261"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{0C938820-B036-4C94-918E-6AB6A9562150}"/>
-    <hyperlink ref="E16" r:id="rId2" xr:uid="{AAC24BC0-DBBD-4BCD-B34D-FBF1CC0F8110}"/>
-    <hyperlink ref="E17" r:id="rId3" xr:uid="{2164CBFD-B0D8-4B90-B5E3-75316CB7E006}"/>
-    <hyperlink ref="E19" r:id="rId4" xr:uid="{6B9C2EB8-FEEB-495A-A221-D466D7F9D741}"/>
-    <hyperlink ref="E18" r:id="rId5" xr:uid="{B52A41F4-FADC-4DEC-9C95-477F1B074EDC}"/>
-    <hyperlink ref="E20" r:id="rId6" xr:uid="{2590EDA3-D089-42AB-8059-AB1A0FA5CEFA}"/>
-    <hyperlink ref="E21" r:id="rId7" location=":~:text=The%20average%20weight%20of%20a%20standard-sized%20or%20multipack,of%20this%20size%20is%20around%20160-180kcal%20per%20pastry." xr:uid="{9A964F89-2A12-42A5-90FA-0EAC39C277DE}"/>
-    <hyperlink ref="E24" r:id="rId8" location=":~:text=The%20average%20weight%20of%20a%20standard-sized%20or%20multipack,of%20this%20size%20is%20around%20160-180kcal%20per%20pastry." xr:uid="{794364C7-3AF3-41FD-BCAE-4DB1EFE46925}"/>
-    <hyperlink ref="E22" r:id="rId9" xr:uid="{D0CD11B2-0B58-482B-A607-EE81764B0A82}"/>
-    <hyperlink ref="E34" r:id="rId10" xr:uid="{A24D2A85-D958-4AFA-A261-CC0A6F4A16BD}"/>
-    <hyperlink ref="E23" r:id="rId11" xr:uid="{AEA0A82A-8A34-414D-99A4-0F035CA44F48}"/>
-    <hyperlink ref="E25" r:id="rId12" xr:uid="{9A08EBA6-AE9F-4B50-896E-5AC5C7DE5269}"/>
-    <hyperlink ref="E26" r:id="rId13" xr:uid="{18CB82EB-27B1-4331-9A1F-A6E553068807}"/>
-    <hyperlink ref="E27" r:id="rId14" xr:uid="{B7D63C53-03DF-4479-822E-BAF53C461B22}"/>
-    <hyperlink ref="E28" r:id="rId15" xr:uid="{A72B9154-4DF9-4EBC-B6B1-623E71795170}"/>
-    <hyperlink ref="E29" r:id="rId16" xr:uid="{2E042FDB-5EDB-4B0B-A8FF-DA750015D9D5}"/>
-    <hyperlink ref="E30" r:id="rId17" xr:uid="{6A53CCF4-E4E4-4406-8A8A-6CABB3C353C3}"/>
-    <hyperlink ref="E31" r:id="rId18" xr:uid="{1FD171DE-5D14-485A-8340-3077327A19C2}"/>
-    <hyperlink ref="E32" r:id="rId19" xr:uid="{539FF15E-BA1D-476A-AC2D-CC7EDDE3D072}"/>
-    <hyperlink ref="E33" r:id="rId20" xr:uid="{A59E57B4-0968-4F8E-99A4-5126F1670304}"/>
-    <hyperlink ref="E35" r:id="rId21" location=":~:text=Weight%20of%20Corn%20on%20the%20Cob%3A%20The%20weight,one%20102g%2F3.6oz%2C%20and%20a%20large%20ear%20about%20143g%2F5oz." xr:uid="{60B0D565-62F2-42C7-A365-31FBD01188BE}"/>
-    <hyperlink ref="E36" r:id="rId22" xr:uid="{B9A67F91-5710-4741-82B0-5D2A967BB937}"/>
-    <hyperlink ref="E37" r:id="rId23" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{08B36A24-C860-41DD-9C6D-4389C469E8E2}"/>
-    <hyperlink ref="E38" r:id="rId24" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{0428D08C-75DB-49E4-A84E-AFB636CEB4F2}"/>
-    <hyperlink ref="E39" r:id="rId25" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{18F9586D-6A0D-4034-AF76-9FADD6F1AFA5}"/>
-    <hyperlink ref="E40" r:id="rId26" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{E37E9319-2C7B-40C3-B805-A6F1F8182919}"/>
-    <hyperlink ref="E41" r:id="rId27" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{BCF694D0-4A1D-451E-B557-CA803EAE9141}"/>
-    <hyperlink ref="E42" r:id="rId28" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{A2409A4D-DF31-4440-8B70-AD6EAB5DF6AA}"/>
-    <hyperlink ref="E43" r:id="rId29" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{A282C59B-FC60-412E-83D6-5823E042A1D5}"/>
-    <hyperlink ref="E44" r:id="rId30" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{DD678B8B-B44C-4CC6-91B5-29D19F2B3934}"/>
-    <hyperlink ref="E45" r:id="rId31" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{38586F0D-3CFB-45C8-9041-DD5C93C066AF}"/>
-    <hyperlink ref="E46" r:id="rId32" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{78644857-D1C0-47DB-A0F1-D6704183408A}"/>
-    <hyperlink ref="E47" r:id="rId33" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{F13294E9-5E90-4F52-AAB7-0138C5DF305B}"/>
-    <hyperlink ref="E48" r:id="rId34" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{EF6FCA90-07B7-4951-BD79-E8E8A9273AEA}"/>
-    <hyperlink ref="E49" r:id="rId35" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{4502A837-5B9F-452D-8AD5-714ED0CBD4E2}"/>
-    <hyperlink ref="E50" r:id="rId36" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{DC54076E-9850-4633-9CB0-257A63CBE999}"/>
-    <hyperlink ref="E51" r:id="rId37" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{82D99C82-2960-4C71-B2A3-C0159047482B}"/>
-    <hyperlink ref="E128" r:id="rId38" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{E77D6CB3-EF4C-4A8D-9B89-E0C400BFF67B}"/>
-    <hyperlink ref="E129" r:id="rId39" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{57D67026-BF79-449B-89BC-8BBB79FA3E39}"/>
-    <hyperlink ref="E130" r:id="rId40" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{F61223EE-9C4B-4EF8-AED2-A86F384BD410}"/>
-    <hyperlink ref="E150" r:id="rId41" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{0EE70D90-B40E-453A-8D12-04E53468FC49}"/>
-    <hyperlink ref="E152" r:id="rId42" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{4F30408C-E3E3-46B1-831A-DAD7684C3D8F}"/>
-    <hyperlink ref="E153" r:id="rId43" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{365293EC-F15A-42AC-9D08-6A16E18F5E00}"/>
-    <hyperlink ref="E154" r:id="rId44" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{E7AB0516-6737-4369-9950-90FB31C52542}"/>
-    <hyperlink ref="E155" r:id="rId45" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{F256DBD7-275A-4037-AA70-E1FDAC3AF475}"/>
-    <hyperlink ref="E156" r:id="rId46" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{E0345A2C-0FB4-4E6D-8383-1F9B2BAE0559}"/>
-    <hyperlink ref="E157" r:id="rId47" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{F52BD257-539D-496D-9884-B2BAC6FFE9CD}"/>
-    <hyperlink ref="E158" r:id="rId48" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{7A05798A-BC66-4FAB-B55C-7AE105F52B88}"/>
-    <hyperlink ref="E159" r:id="rId49" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{94EC17A4-D1F1-4E8C-BF18-DA0A4382AE40}"/>
-    <hyperlink ref="E160" r:id="rId50" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{0A2A7360-BE55-4CC3-B77A-0B2816E50A09}"/>
-    <hyperlink ref="E162" r:id="rId51" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{BB4DCFBB-29A3-45D0-A5AA-1560D4308A2E}"/>
-    <hyperlink ref="E163" r:id="rId52" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{2ED29159-F7A5-4353-8B88-367AF54CCBF9}"/>
-    <hyperlink ref="E164" r:id="rId53" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{1C293D6D-D2AF-4855-B4F6-0D9C7016EA38}"/>
-    <hyperlink ref="E195" r:id="rId54" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{E6ACCB3F-20BF-4E95-8A5F-011301046C84}"/>
-    <hyperlink ref="E196" r:id="rId55" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{50A76BB9-ED8D-4964-B3E7-A65A4D48D847}"/>
-    <hyperlink ref="E253" r:id="rId56" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{4F52EDE4-53A8-40B8-9531-378FDA37D409}"/>
-    <hyperlink ref="E254" r:id="rId57" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{B8E86C3B-28E4-47B0-B609-46F339957735}"/>
-    <hyperlink ref="E255" r:id="rId58" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{AF50DC4B-2BCF-4311-A76D-6AE2C6AAEB18}"/>
-    <hyperlink ref="E256" r:id="rId59" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{EBFBDE99-A3EB-4270-91DC-558DA0216700}"/>
-    <hyperlink ref="E257" r:id="rId60" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{611D8602-9FAB-45D2-A70D-D1CBF6297FC3}"/>
-    <hyperlink ref="E54" r:id="rId61" xr:uid="{4CF870C7-083F-438B-8876-EA8CA1A3F8B9}"/>
-    <hyperlink ref="E53" r:id="rId62" xr:uid="{D11C496C-3A8D-4FFF-917D-9FD9C835289E}"/>
-    <hyperlink ref="E52" r:id="rId63" xr:uid="{C0C78CEC-AD21-486E-9B63-33872B99DBA4}"/>
-    <hyperlink ref="E55" r:id="rId64" xr:uid="{91096BC4-0126-4316-B62B-7301585DF7ED}"/>
-    <hyperlink ref="E56" r:id="rId65" xr:uid="{B2C81A33-8F2B-4C38-B9D1-21C33B9710AD}"/>
-    <hyperlink ref="E57" r:id="rId66" xr:uid="{141916A2-8C14-4F77-A8BB-F85A2A2E3725}"/>
-    <hyperlink ref="E58" r:id="rId67" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae.750" xr:uid="{A3B2B655-6B14-491C-9A7B-96C920A1E825}"/>
-    <hyperlink ref="E59" r:id="rId68" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae.750" xr:uid="{387EA55F-B920-4199-94E0-A4DF9E93B4E6}"/>
-    <hyperlink ref="E60" r:id="rId69" xr:uid="{0C62E57E-4669-4187-9CAA-4D6C7C81C1E6}"/>
-    <hyperlink ref="E61" r:id="rId70" xr:uid="{BD3ACFAA-54B0-4440-A2E1-D3616C799B10}"/>
-    <hyperlink ref="E62" r:id="rId71" xr:uid="{58E8B664-9FDA-4BDC-A414-E1FBB997A08D}"/>
-    <hyperlink ref="E63" r:id="rId72" xr:uid="{30FA0E86-6C91-4B45-A62C-392EC0DCAE48}"/>
-    <hyperlink ref="E64" r:id="rId73" xr:uid="{A7055CC2-5123-4E1B-AE43-588096CC5814}"/>
-    <hyperlink ref="E65" r:id="rId74" xr:uid="{71922CAD-E104-4B11-8918-859962B215E3}"/>
-    <hyperlink ref="E67" r:id="rId75" xr:uid="{573FCB46-3B08-426B-BE9D-5314FFE380A8}"/>
-    <hyperlink ref="E66" r:id="rId76" xr:uid="{1543F6F8-5D90-4163-960D-9EE47CCB6071}"/>
-    <hyperlink ref="E68:E69" r:id="rId77" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{27D59C05-B58B-4EAD-960C-CC3D2421576A}"/>
-    <hyperlink ref="E68" r:id="rId78" xr:uid="{EE29AE06-087B-45FE-9A6B-AEFFA885E341}"/>
-    <hyperlink ref="E71" r:id="rId79" xr:uid="{B2A6033D-16A2-449A-924B-EC58C01A017C}"/>
-    <hyperlink ref="E70" r:id="rId80" xr:uid="{55A0A422-4341-432B-B1B5-2E80D6447FFB}"/>
-    <hyperlink ref="E72:E73" r:id="rId81" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{EA3DD48B-B724-49E8-A457-D6C85047F263}"/>
-    <hyperlink ref="E78:E79" r:id="rId82" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{50B383A9-BAA6-435B-94B8-522EE3A003F3}"/>
-    <hyperlink ref="E74:E75" r:id="rId83" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{5DD7AA27-B6DE-42FA-80D1-8FE33092D073}"/>
-    <hyperlink ref="E76:E77" r:id="rId84" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{316AC6D6-8589-450D-8519-4B4C73A8F1D0}"/>
-    <hyperlink ref="E80:E81" r:id="rId85" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{54243E60-85F2-42CA-8B67-486103D58F0F}"/>
-    <hyperlink ref="E82" r:id="rId86" xr:uid="{8B1FFEE0-5F17-4D54-B328-0F6E0BED72BC}"/>
-    <hyperlink ref="E83" r:id="rId87" xr:uid="{C5F55AD2-43FD-4BCA-B75B-1926BC89480F}"/>
-    <hyperlink ref="E84" r:id="rId88" xr:uid="{B064DC33-A7D4-4DA1-99AA-2D036A2371B6}"/>
-    <hyperlink ref="E85" r:id="rId89" xr:uid="{E0BADBF2-950C-43AA-972C-2E7F5C7F29C6}"/>
-    <hyperlink ref="E86" r:id="rId90" display="https://www.bing.com/ck/a?!&amp;&amp;p=8ec6058a341582cdJmltdHM9MTcwOTY4MzIwMCZpZ3VpZD0zMjYyNDYwOS04MzdjLTYyNjYtMTAxYS01N2U2ODJkMzYzOTMmaW5zaWQ9NTUyNA&amp;ptn=3&amp;ver=2&amp;hsh=3&amp;fclid=32624609-837c-6266-101a-57e682d36393&amp;psq=vining+tomato+average+weight&amp;u=a1aHR0cHM6Ly93d3cubXlnYXJkZW4uY29tL2dhcnRlbnByYXhpcy9udXR6Z2FydGVuL3ZpbmUtdG9tYXRvZXMtYmVzdC12YXJpZXRpZXMtMzc2NzYjOn46dGV4dD1JdHMlMjBmcnVpdHMlMjB3ZWlnaCx1cCUyMHRvJTIwMy41MyUyMG91bmNlcy4&amp;ntb=1" xr:uid="{D224D88F-9EA3-4C7C-8386-AD0CA3B7C0E6}"/>
-    <hyperlink ref="E87" r:id="rId91" location=":~:text=So%2C%20how%20much%20do%20onions%20weigh%3F%20A%20small,onion%20will%20weigh%20around%205.29%20ounces%20%28150%20grams%29." xr:uid="{99C54A81-544D-49B6-9020-6DE16C097E00}"/>
-    <hyperlink ref="E88" r:id="rId92" location=":~:text=On%20average%2C%20a%20leek%20weighs%20about%20200-300%20grams,or%20as%20much%20as%20500%20grams%20%2817.6%20ounces%29." xr:uid="{FA6388F7-452F-4452-9DD3-85F8EAE94188}"/>
-    <hyperlink ref="E89" r:id="rId93" xr:uid="{617775D9-C8F5-4928-85B9-2AA88A08ED62}"/>
-    <hyperlink ref="E90" r:id="rId94" xr:uid="{CD58460A-9C1E-4BD7-8DAC-3A0F6F4839E1}"/>
-    <hyperlink ref="E92" r:id="rId95" xr:uid="{8E2EE6B8-51EF-4106-82B3-246F7D0126C7}"/>
-    <hyperlink ref="E91" r:id="rId96" xr:uid="{59471633-01B8-4CC0-AD0E-F11ABDFB48C5}"/>
-    <hyperlink ref="E93" r:id="rId97" xr:uid="{C5147F4A-7D4B-463B-B697-A97179B3E947}"/>
-    <hyperlink ref="E94" r:id="rId98" xr:uid="{5F506CD0-8675-44A1-9D44-2810CE0EBE55}"/>
-    <hyperlink ref="E95" r:id="rId99" xr:uid="{0D976289-5324-43E7-A529-F55DE5EC7C36}"/>
-    <hyperlink ref="E96" r:id="rId100" xr:uid="{E658BFCB-B035-4FA1-8298-2C642D509D65}"/>
-    <hyperlink ref="E97" r:id="rId101" xr:uid="{ABDC1D17-9E06-4A6E-86C8-1F19B76FF457}"/>
-    <hyperlink ref="E98" r:id="rId102" xr:uid="{B494CEBD-EBD6-482F-A6DF-EFBA1F71B016}"/>
-    <hyperlink ref="E99" r:id="rId103" xr:uid="{F4FA55AB-0EB9-4579-BE57-4DA79D440BCE}"/>
-    <hyperlink ref="E100" r:id="rId104" location=":~:text=A%20whole%20artichoke%20can%20weigh%20anywhere%20between%205,14%20to%2016%20ounces%20%28400%20to%20450%20grams%29." xr:uid="{161CDFC2-F672-41BF-8BCA-AB52AD1D35E5}"/>
-    <hyperlink ref="E103" r:id="rId105" xr:uid="{E3AE809E-882D-4CF2-B11B-0FD473A58D4C}"/>
-    <hyperlink ref="E108" r:id="rId106" xr:uid="{F06CCB42-333B-4E30-8C23-6FCFF3B49CD3}"/>
-    <hyperlink ref="E109" r:id="rId107" xr:uid="{6253898E-66C4-4554-B9D7-3F86F09D71D9}"/>
-    <hyperlink ref="E102" r:id="rId108" xr:uid="{4C459FFB-56E0-4B6C-A2E4-C99A118705CC}"/>
-    <hyperlink ref="E104" r:id="rId109" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae." xr:uid="{9777807A-B6B9-4C93-BEF4-BEFC47DE2A4C}"/>
-    <hyperlink ref="E110" r:id="rId110" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae." xr:uid="{1845F127-ACA8-48EB-A292-77C1EA965FD5}"/>
-    <hyperlink ref="E105" r:id="rId111" location=":~:text=With%20a%20weight%20of%20two%20to%20four%20pounds%2C,them%20an%20especially%20good%20option%20for%20pumpkin%20soup." xr:uid="{FC33E91A-F3A5-44BA-8053-44CBA17D05EC}"/>
-    <hyperlink ref="E106" r:id="rId112" location=":~:text=Understanding%20the%20Weight%20of%20Iceberg%20Lettuce%20A%20head,on%20the%20size%20and%20density%20of%20the%20head." xr:uid="{73192AC7-4606-41E7-894B-0CF48E9CD241}"/>
-    <hyperlink ref="E107" r:id="rId113" xr:uid="{CB380595-D555-4174-BB03-09EEE5B9D47D}"/>
-    <hyperlink ref="E101" r:id="rId114" xr:uid="{56649441-CFD7-4967-83FC-BA5CC862FC38}"/>
-    <hyperlink ref="E127" r:id="rId115" xr:uid="{FB499B0E-9651-4A80-AFAC-2343FAD8C218}"/>
-    <hyperlink ref="E126" r:id="rId116" xr:uid="{FFBC87F3-5CD4-46D5-9E5D-FC38936777D3}"/>
-    <hyperlink ref="E122" r:id="rId117" xr:uid="{D5BEF76D-509C-4A5D-8CF3-B0149F37C3AE}"/>
-    <hyperlink ref="E125" r:id="rId118" xr:uid="{DF96B31C-D8D1-4B2F-8330-E961C0D7AA3E}"/>
-    <hyperlink ref="E124" r:id="rId119" location=":~:text=The%20weight%20of%20an%20orange%20mostly%20depends%20on,can%20weigh%20up%20to%20300%20grams%20or%20more." xr:uid="{7D879F44-D043-4305-9CD1-18B6FB2BAD75}"/>
-    <hyperlink ref="E123" r:id="rId120" location=":~:text=The%20average%20weight%20of%20one%20Mandarin%20%28also%20known,or%20clementine%29%20weighs%20around%20100-110g%20including%20the%20peel." xr:uid="{9130A100-A675-4C6B-BF9E-4962A830C67C}"/>
-    <hyperlink ref="E121" r:id="rId121" location=":~:text=The%20average%20weight%20of%20one%20Mandarin%20%28also%20known,or%20clementine%29%20weighs%20around%20100-110g%20including%20the%20peel." xr:uid="{0214FFCD-260C-4CAC-98A6-9E7BF8727EC9}"/>
-    <hyperlink ref="E120" r:id="rId122" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae." xr:uid="{0493224D-F634-4DC9-B8F5-D23DE9ABCFC5}"/>
-    <hyperlink ref="E118" r:id="rId123" xr:uid="{FEA3894E-E270-4A86-B49B-9417C6DB019B}"/>
-    <hyperlink ref="E119" r:id="rId124" location=":~:text=The%20weight%20of%20an%20orange%20mostly%20depends%20on,can%20weigh%20up%20to%20300%20grams%20or%20more." xr:uid="{C1AADE4E-E45D-4341-B5AE-10BD7A5E8158}"/>
-    <hyperlink ref="E131" r:id="rId125" xr:uid="{DB5256D4-2794-4DA7-9860-58586D85C842}"/>
-    <hyperlink ref="E134" r:id="rId126" xr:uid="{4C57A8E7-B979-4AC9-A9EE-BEFBB86C8A22}"/>
-    <hyperlink ref="E133" r:id="rId127" xr:uid="{96DB25E4-C54B-41EA-BE91-D02B2B923AFD}"/>
-    <hyperlink ref="E132" r:id="rId128" location=":~:text=It%20is%20native%20to%20North%20America%20and%20is,yellow%20and%20offers%20a%20juicy%20sweetness%20when%20eaten." xr:uid="{28F03024-2BF3-4F9A-88CD-DD6BB3A78E49}"/>
-    <hyperlink ref="E136" r:id="rId129" xr:uid="{9838061A-9059-4F00-9FF1-7CE25601BDBF}"/>
-    <hyperlink ref="E135" r:id="rId130" location=":~:text=Melon%20%28cantaloupe%29%201%203%20lbs.%201.36,kg%20Melon%20%28honeydew%29%201%204%20lbs." xr:uid="{F8ADD103-5E05-451E-B856-880D71CB3995}"/>
-    <hyperlink ref="E139" r:id="rId131" xr:uid="{77B75B22-AFEB-4F1F-8427-050F0FA591C8}"/>
-    <hyperlink ref="E138" r:id="rId132" xr:uid="{6914D4FD-7F7C-4E6E-ADD7-558390155AE8}"/>
-    <hyperlink ref="E141" r:id="rId133" xr:uid="{7F7F684E-CD6C-45E4-9DFB-4BABAC6E9D77}"/>
-    <hyperlink ref="E142" r:id="rId134" xr:uid="{0875C14F-EE18-4D2C-9803-EF2ED87440C3}"/>
-    <hyperlink ref="E140" r:id="rId135" xr:uid="{54A67086-9136-4E91-8F5C-77CA94FC4295}"/>
-    <hyperlink ref="E166" r:id="rId136" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{DB9CB5D9-B953-4199-B703-0B864098AF53}"/>
-    <hyperlink ref="E167" r:id="rId137" location=":~:text=One%20whole%20chicken%20egg%20weighs%20an%20average%20of,of%20nutritional%20value%2C%20and%20the%20lowest%20in%20cholesterol." xr:uid="{9CF2F174-6FE7-469E-9FB9-7E95AD8C899F}"/>
-    <hyperlink ref="E172:E173" r:id="rId138" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{CF387F13-7B29-4B55-AD23-51C4FD578AE8}"/>
-    <hyperlink ref="E183:E184" r:id="rId139" display="https://www.omnicalculator.com/conversion/tbsp-to-grams" xr:uid="{8BA7D8A2-7199-45F1-9E16-672BC959CA73}"/>
-    <hyperlink ref="E219" r:id="rId140" location=":~:text=A%20typical%20garlic%20clove%20usually%20weighs%20between%203,that%20have%20been%20sitting%20around%20for%20a%20while." xr:uid="{18D2F62F-5E96-4336-9D6D-C69930F6E3B3}"/>
-    <hyperlink ref="E182" r:id="rId141" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{3C2EA481-2BA5-4F1A-9052-2937FAE3AFBD}"/>
-    <hyperlink ref="E252" r:id="rId142" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{757A1EBC-D5E1-4C42-B4F4-4990F11501AC}"/>
-    <hyperlink ref="E259" r:id="rId143" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." xr:uid="{72FC6F6B-FA26-47DD-90E7-8C78F703D5D7}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E16" r:id="rId2"/>
+    <hyperlink ref="E17" r:id="rId3"/>
+    <hyperlink ref="E19" r:id="rId4"/>
+    <hyperlink ref="E18" r:id="rId5"/>
+    <hyperlink ref="E20" r:id="rId6"/>
+    <hyperlink ref="E21" r:id="rId7" location=":~:text=The%20average%20weight%20of%20a%20standard-sized%20or%20multipack,of%20this%20size%20is%20around%20160-180kcal%20per%20pastry."/>
+    <hyperlink ref="E24" r:id="rId8" location=":~:text=The%20average%20weight%20of%20a%20standard-sized%20or%20multipack,of%20this%20size%20is%20around%20160-180kcal%20per%20pastry."/>
+    <hyperlink ref="E22" r:id="rId9"/>
+    <hyperlink ref="E34" r:id="rId10"/>
+    <hyperlink ref="E23" r:id="rId11"/>
+    <hyperlink ref="E25" r:id="rId12"/>
+    <hyperlink ref="E26" r:id="rId13"/>
+    <hyperlink ref="E27" r:id="rId14"/>
+    <hyperlink ref="E28" r:id="rId15"/>
+    <hyperlink ref="E29" r:id="rId16"/>
+    <hyperlink ref="E30" r:id="rId17"/>
+    <hyperlink ref="E31" r:id="rId18"/>
+    <hyperlink ref="E32" r:id="rId19"/>
+    <hyperlink ref="E33" r:id="rId20"/>
+    <hyperlink ref="E35" r:id="rId21" location=":~:text=Weight%20of%20Corn%20on%20the%20Cob%3A%20The%20weight,one%20102g%2F3.6oz%2C%20and%20a%20large%20ear%20about%20143g%2F5oz."/>
+    <hyperlink ref="E36" r:id="rId22"/>
+    <hyperlink ref="E37" r:id="rId23" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E38" r:id="rId24" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E39" r:id="rId25" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E40" r:id="rId26" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E41" r:id="rId27" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E42" r:id="rId28" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E43" r:id="rId29" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E44" r:id="rId30" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E45" r:id="rId31" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E46" r:id="rId32" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E47" r:id="rId33" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E48" r:id="rId34" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E49" r:id="rId35" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E50" r:id="rId36" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E51" r:id="rId37" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E128" r:id="rId38" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E129" r:id="rId39" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E130" r:id="rId40" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E150" r:id="rId41" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E152" r:id="rId42" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E153" r:id="rId43" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E154" r:id="rId44" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E155" r:id="rId45" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E156" r:id="rId46" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E158" r:id="rId47" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E159" r:id="rId48" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E160" r:id="rId49" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E192" r:id="rId50" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E193" r:id="rId51" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E254" r:id="rId52" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E255" r:id="rId53" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E256" r:id="rId54" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E257" r:id="rId55" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E258" r:id="rId56" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E54" r:id="rId57"/>
+    <hyperlink ref="E53" r:id="rId58"/>
+    <hyperlink ref="E52" r:id="rId59"/>
+    <hyperlink ref="E55" r:id="rId60"/>
+    <hyperlink ref="E56" r:id="rId61"/>
+    <hyperlink ref="E57" r:id="rId62"/>
+    <hyperlink ref="E58" r:id="rId63" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae.750"/>
+    <hyperlink ref="E59" r:id="rId64" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae.750"/>
+    <hyperlink ref="E60" r:id="rId65"/>
+    <hyperlink ref="E61" r:id="rId66"/>
+    <hyperlink ref="E62" r:id="rId67"/>
+    <hyperlink ref="E63" r:id="rId68"/>
+    <hyperlink ref="E64" r:id="rId69"/>
+    <hyperlink ref="E65" r:id="rId70"/>
+    <hyperlink ref="E67" r:id="rId71"/>
+    <hyperlink ref="E66" r:id="rId72"/>
+    <hyperlink ref="E68:E69" r:id="rId73" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E68" r:id="rId74"/>
+    <hyperlink ref="E71" r:id="rId75"/>
+    <hyperlink ref="E70" r:id="rId76"/>
+    <hyperlink ref="E72:E73" r:id="rId77" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E78:E79" r:id="rId78" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E74:E75" r:id="rId79" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E76:E77" r:id="rId80" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E80:E81" r:id="rId81" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E82" r:id="rId82"/>
+    <hyperlink ref="E83" r:id="rId83"/>
+    <hyperlink ref="E84" r:id="rId84"/>
+    <hyperlink ref="E85" r:id="rId85"/>
+    <hyperlink ref="E86" r:id="rId86" display="https://www.bing.com/ck/a?!&amp;&amp;p=8ec6058a341582cdJmltdHM9MTcwOTY4MzIwMCZpZ3VpZD0zMjYyNDYwOS04MzdjLTYyNjYtMTAxYS01N2U2ODJkMzYzOTMmaW5zaWQ9NTUyNA&amp;ptn=3&amp;ver=2&amp;hsh=3&amp;fclid=32624609-837c-6266-101a-57e682d36393&amp;psq=vining+tomato+average+weight&amp;u=a1aHR0cHM6Ly93d3cubXlnYXJkZW4uY29tL2dhcnRlbnByYXhpcy9udXR6Z2FydGVuL3ZpbmUtdG9tYXRvZXMtYmVzdC12YXJpZXRpZXMtMzc2NzYjOn46dGV4dD1JdHMlMjBmcnVpdHMlMjB3ZWlnaCx1cCUyMHRvJTIwMy41MyUyMG91bmNlcy4&amp;ntb=1"/>
+    <hyperlink ref="E87" r:id="rId87" location=":~:text=So%2C%20how%20much%20do%20onions%20weigh%3F%20A%20small,onion%20will%20weigh%20around%205.29%20ounces%20%28150%20grams%29."/>
+    <hyperlink ref="E88" r:id="rId88" location=":~:text=On%20average%2C%20a%20leek%20weighs%20about%20200-300%20grams,or%20as%20much%20as%20500%20grams%20%2817.6%20ounces%29."/>
+    <hyperlink ref="E89" r:id="rId89"/>
+    <hyperlink ref="E90" r:id="rId90"/>
+    <hyperlink ref="E92" r:id="rId91"/>
+    <hyperlink ref="E91" r:id="rId92"/>
+    <hyperlink ref="E93" r:id="rId93"/>
+    <hyperlink ref="E94" r:id="rId94"/>
+    <hyperlink ref="E95" r:id="rId95"/>
+    <hyperlink ref="E96" r:id="rId96"/>
+    <hyperlink ref="E97" r:id="rId97"/>
+    <hyperlink ref="E98" r:id="rId98"/>
+    <hyperlink ref="E99" r:id="rId99"/>
+    <hyperlink ref="E100" r:id="rId100" location=":~:text=A%20whole%20artichoke%20can%20weigh%20anywhere%20between%205,14%20to%2016%20ounces%20%28400%20to%20450%20grams%29."/>
+    <hyperlink ref="E103" r:id="rId101"/>
+    <hyperlink ref="E108" r:id="rId102"/>
+    <hyperlink ref="E109" r:id="rId103"/>
+    <hyperlink ref="E102" r:id="rId104"/>
+    <hyperlink ref="E104" r:id="rId105" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae."/>
+    <hyperlink ref="E110" r:id="rId106" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae."/>
+    <hyperlink ref="E105" r:id="rId107" location=":~:text=With%20a%20weight%20of%20two%20to%20four%20pounds%2C,them%20an%20especially%20good%20option%20for%20pumpkin%20soup."/>
+    <hyperlink ref="E106" r:id="rId108" location=":~:text=Understanding%20the%20Weight%20of%20Iceberg%20Lettuce%20A%20head,on%20the%20size%20and%20density%20of%20the%20head."/>
+    <hyperlink ref="E107" r:id="rId109"/>
+    <hyperlink ref="E101" r:id="rId110"/>
+    <hyperlink ref="E127" r:id="rId111"/>
+    <hyperlink ref="E126" r:id="rId112"/>
+    <hyperlink ref="E122" r:id="rId113"/>
+    <hyperlink ref="E125" r:id="rId114"/>
+    <hyperlink ref="E124" r:id="rId115" location=":~:text=The%20weight%20of%20an%20orange%20mostly%20depends%20on,can%20weigh%20up%20to%20300%20grams%20or%20more."/>
+    <hyperlink ref="E123" r:id="rId116" location=":~:text=The%20average%20weight%20of%20one%20Mandarin%20%28also%20known,or%20clementine%29%20weighs%20around%20100-110g%20including%20the%20peel."/>
+    <hyperlink ref="E121" r:id="rId117" location=":~:text=The%20average%20weight%20of%20one%20Mandarin%20%28also%20known,or%20clementine%29%20weighs%20around%20100-110g%20including%20the%20peel."/>
+    <hyperlink ref="E120" r:id="rId118" location=":~:text=0.7%20kg%20%281.5%20lbs.%29%20Citruses%20Citrus%20fruit%20is,fruit%20that%20belongs%20to%20the%20family%20of%20Rutaceae."/>
+    <hyperlink ref="E118" r:id="rId119"/>
+    <hyperlink ref="E119" r:id="rId120" location=":~:text=The%20weight%20of%20an%20orange%20mostly%20depends%20on,can%20weigh%20up%20to%20300%20grams%20or%20more."/>
+    <hyperlink ref="E131" r:id="rId121"/>
+    <hyperlink ref="E134" r:id="rId122"/>
+    <hyperlink ref="E133" r:id="rId123"/>
+    <hyperlink ref="E132" r:id="rId124" location=":~:text=It%20is%20native%20to%20North%20America%20and%20is,yellow%20and%20offers%20a%20juicy%20sweetness%20when%20eaten."/>
+    <hyperlink ref="E136" r:id="rId125"/>
+    <hyperlink ref="E135" r:id="rId126" location=":~:text=Melon%20%28cantaloupe%29%201%203%20lbs.%201.36,kg%20Melon%20%28honeydew%29%201%204%20lbs."/>
+    <hyperlink ref="E139" r:id="rId127"/>
+    <hyperlink ref="E138" r:id="rId128"/>
+    <hyperlink ref="E141" r:id="rId129"/>
+    <hyperlink ref="E142" r:id="rId130"/>
+    <hyperlink ref="E140" r:id="rId131"/>
+    <hyperlink ref="E162" r:id="rId132" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E163" r:id="rId133" location=":~:text=One%20whole%20chicken%20egg%20weighs%20an%20average%20of,of%20nutritional%20value%2C%20and%20the%20lowest%20in%20cholesterol."/>
+    <hyperlink ref="E168:E169" r:id="rId134" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E180:E181" r:id="rId135" display="https://www.omnicalculator.com/conversion/tbsp-to-grams"/>
+    <hyperlink ref="E217" r:id="rId136" location=":~:text=A%20typical%20garlic%20clove%20usually%20weighs%20between%203,that%20have%20been%20sitting%20around%20for%20a%20while."/>
+    <hyperlink ref="E178" r:id="rId137" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E253" r:id="rId138" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E261" r:id="rId139" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
+    <hyperlink ref="E250:E252" r:id="rId140" location=":~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions." display="https://www.convertunits.com/from/deciliters/to/grams#:~:text=Do%20a%20quick%20conversion%3A%201%20deciliters%20%3D%20100,grams%20using%20the%20online%20calculator%20for%20metric%20conversions."/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId144"/>
+  <legacyDrawing r:id="rId141"/>
 </worksheet>
 </file>
</xml_diff>